<commit_message>
overwrite SYVBT to calibrate vehicle #s
</commit_message>
<xml_diff>
--- a/InputData/trans/SYVbT/Start Year Vehicles by Technology.xlsx
+++ b/InputData/trans/SYVbT/Start Year Vehicles by Technology.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lainie Rowland\Desktop\GitHub Repos\state-eps-data-repository\NY\trans\SYVbT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lainie Rowland\Desktop\GitHub Repos\eps-newyork\InputData\trans\SYVbT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{780588F1-D3A5-4BE4-982D-37F1887C8D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC24F712-0CF9-4E20-837F-5C02FB695429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1520" windowWidth="10800" windowHeight="8840" firstSheet="11" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="13" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -4375,34 +4375,55 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -4412,41 +4433,20 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="143">
@@ -6423,8 +6423,8 @@
   </sheetPr>
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -6469,30 +6469,24 @@
         <v>2</v>
       </c>
       <c r="B2" s="18">
-        <f>ROUND('USA Values'!B3*'Share of VT by state'!$B$2,0)</f>
-        <v>35955</v>
+        <v>23588.010515924994</v>
       </c>
       <c r="C2" s="18">
         <v>0</v>
       </c>
       <c r="D2" s="18">
-        <f>ROUND('USA Values'!D3*'Share of VT by state'!$B$2,0)</f>
-        <v>15849763</v>
+        <v>10398119.213431202</v>
       </c>
       <c r="E2" s="18">
-        <f>ROUND('USA Values'!E3*'Share of VT by state'!$B$2,0)</f>
-        <v>79745</v>
+        <v>52316.114548531186</v>
       </c>
       <c r="F2" s="18">
-        <f>ROUND('USA Values'!F3*'Share of VT by state'!$B$2,0)</f>
-        <v>33355</v>
+        <v>21882.29984031924</v>
       </c>
       <c r="G2" s="18">
-        <f>ROUND('USA Values'!G3*'Share of VT by state'!$B$2,0)</f>
-        <v>6241</v>
+        <v>4094.3616640213572</v>
       </c>
       <c r="H2" s="18">
-        <f>ROUND('USA Values'!H3*'Share of VT by state'!$B$2,0)</f>
         <v>0</v>
       </c>
       <c r="J2" s="18"/>
@@ -6656,8 +6650,8 @@
   </sheetPr>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -6703,29 +6697,24 @@
         <v>2</v>
       </c>
       <c r="B2" s="18">
-        <f>ROUND('USA Values'!B12*'Share of VT by state'!$B$4,0)</f>
         <v>0</v>
       </c>
       <c r="C2" s="18">
         <v>0</v>
       </c>
       <c r="D2" s="18">
-        <f>SUM(ROUND('USA Values'!D12*'Share of VT by state'!$B$4,0),ROUND('USA Values'!D13*'Share of VT by state'!$B$5,0))</f>
-        <v>724649</v>
+        <v>201233.5032021653</v>
       </c>
       <c r="E2" s="18">
         <v>0</v>
       </c>
       <c r="F2" s="18">
-        <f>ROUND('USA Values'!F12*'Share of VT by state'!$B$4,0)</f>
         <v>0</v>
       </c>
       <c r="G2" s="18">
-        <f>ROUND('USA Values'!G12*'Share of VT by state'!$B$4,0)</f>
-        <v>44</v>
+        <v>12.21870745822498</v>
       </c>
       <c r="H2" s="18">
-        <f>ROUND('USA Values'!H12*'Share of VT by state'!$B$4,0)</f>
         <v>0</v>
       </c>
       <c r="I2" s="67"/>
@@ -6735,30 +6724,25 @@
       <c r="A3" s="1" t="s">
         <v>1077</v>
       </c>
-      <c r="B3">
-        <f>ROUND('USA Values'!B13*'Share of VT by state'!$B$5,0)</f>
-        <v>197</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <f>SUM(ROUND('USA Values'!E13*'Share of VT by state'!$B$5,0),ROUND('USA Values'!E12*'Share of VT by state'!$B$4,0))</f>
-        <v>895019</v>
-      </c>
-      <c r="F3">
-        <f>ROUND('USA Values'!F13*'Share of VT by state'!$B$5,0)</f>
-        <v>80</v>
-      </c>
-      <c r="G3">
-        <f>ROUND('USA Values'!G13*'Share of VT by state'!$B$5,0)</f>
-        <v>477</v>
-      </c>
-      <c r="H3">
-        <f>ROUND('USA Values'!H13*'Share of VT by state'!$B$5,0)</f>
+      <c r="B3" s="18">
+        <v>54.706485665234574</v>
+      </c>
+      <c r="C3" s="18">
+        <v>0</v>
+      </c>
+      <c r="D3" s="18">
+        <v>0</v>
+      </c>
+      <c r="E3" s="18">
+        <v>248544.89387620596</v>
+      </c>
+      <c r="F3" s="18">
+        <v>22.215831742227234</v>
+      </c>
+      <c r="G3" s="18">
+        <v>132.4618967630299</v>
+      </c>
+      <c r="H3" s="18">
         <v>0</v>
       </c>
       <c r="J3" s="18"/>
@@ -79763,43 +79747,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="93" t="s">
         <v>928</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="87"/>
-      <c r="O1" s="87"/>
-      <c r="P1" s="87"/>
-      <c r="Q1" s="87"/>
-      <c r="R1" s="87"/>
-      <c r="S1" s="87"/>
-      <c r="T1" s="87"/>
-      <c r="U1" s="87"/>
-      <c r="V1" s="87"/>
-      <c r="W1" s="87"/>
-      <c r="X1" s="87"/>
-      <c r="Y1" s="87"/>
-      <c r="Z1" s="87"/>
-      <c r="AA1" s="87"/>
-      <c r="AB1" s="87"/>
-      <c r="AC1" s="87"/>
-      <c r="AD1" s="87"/>
-      <c r="AE1" s="87"/>
-      <c r="AF1" s="87"/>
-      <c r="AG1" s="87"/>
-      <c r="AH1" s="87"/>
-      <c r="AI1" s="87"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="94"/>
+      <c r="J1" s="94"/>
+      <c r="K1" s="94"/>
+      <c r="L1" s="94"/>
+      <c r="M1" s="94"/>
+      <c r="N1" s="94"/>
+      <c r="O1" s="94"/>
+      <c r="P1" s="94"/>
+      <c r="Q1" s="94"/>
+      <c r="R1" s="94"/>
+      <c r="S1" s="94"/>
+      <c r="T1" s="94"/>
+      <c r="U1" s="94"/>
+      <c r="V1" s="94"/>
+      <c r="W1" s="94"/>
+      <c r="X1" s="94"/>
+      <c r="Y1" s="94"/>
+      <c r="Z1" s="94"/>
+      <c r="AA1" s="94"/>
+      <c r="AB1" s="94"/>
+      <c r="AC1" s="94"/>
+      <c r="AD1" s="94"/>
+      <c r="AE1" s="94"/>
+      <c r="AF1" s="94"/>
+      <c r="AG1" s="94"/>
+      <c r="AH1" s="94"/>
+      <c r="AI1" s="94"/>
     </row>
     <row r="2" spans="1:37" s="19" customFormat="1" ht="16.5" customHeight="1">
       <c r="A2" s="31"/>
@@ -83063,26 +83047,26 @@
       </c>
     </row>
     <row r="35" spans="1:35" s="72" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A35" s="88" t="s">
+      <c r="A35" s="95" t="s">
         <v>963</v>
       </c>
-      <c r="B35" s="89"/>
-      <c r="C35" s="89"/>
-      <c r="D35" s="89"/>
-      <c r="E35" s="89"/>
-      <c r="F35" s="89"/>
-      <c r="G35" s="89"/>
-      <c r="H35" s="89"/>
-      <c r="I35" s="89"/>
-      <c r="J35" s="89"/>
-      <c r="K35" s="89"/>
-      <c r="L35" s="89"/>
-      <c r="M35" s="89"/>
-      <c r="N35" s="89"/>
-      <c r="O35" s="89"/>
-      <c r="P35" s="89"/>
-      <c r="Q35" s="89"/>
-      <c r="R35" s="89"/>
+      <c r="B35" s="96"/>
+      <c r="C35" s="96"/>
+      <c r="D35" s="96"/>
+      <c r="E35" s="96"/>
+      <c r="F35" s="96"/>
+      <c r="G35" s="96"/>
+      <c r="H35" s="96"/>
+      <c r="I35" s="96"/>
+      <c r="J35" s="96"/>
+      <c r="K35" s="96"/>
+      <c r="L35" s="96"/>
+      <c r="M35" s="96"/>
+      <c r="N35" s="96"/>
+      <c r="O35" s="96"/>
+      <c r="P35" s="96"/>
+      <c r="Q35" s="96"/>
+      <c r="R35" s="96"/>
       <c r="S35" s="54"/>
       <c r="T35" s="54"/>
       <c r="U35" s="54"/>
@@ -83098,26 +83082,26 @@
     </row>
     <row r="36" spans="1:35" s="72" customFormat="1" ht="12.75" customHeight="1">
       <c r="A36" s="90"/>
-      <c r="B36" s="91"/>
-      <c r="C36" s="91"/>
-      <c r="D36" s="91"/>
-      <c r="E36" s="91"/>
-      <c r="F36" s="91"/>
-      <c r="G36" s="91"/>
-      <c r="H36" s="91"/>
-      <c r="I36" s="91"/>
-      <c r="J36" s="91"/>
-      <c r="K36" s="91"/>
-      <c r="L36" s="91"/>
-      <c r="M36" s="91"/>
-      <c r="N36" s="91"/>
-      <c r="O36" s="91"/>
-      <c r="P36" s="91"/>
-      <c r="Q36" s="91"/>
-      <c r="R36" s="91"/>
+      <c r="B36" s="97"/>
+      <c r="C36" s="97"/>
+      <c r="D36" s="97"/>
+      <c r="E36" s="97"/>
+      <c r="F36" s="97"/>
+      <c r="G36" s="97"/>
+      <c r="H36" s="97"/>
+      <c r="I36" s="97"/>
+      <c r="J36" s="97"/>
+      <c r="K36" s="97"/>
+      <c r="L36" s="97"/>
+      <c r="M36" s="97"/>
+      <c r="N36" s="97"/>
+      <c r="O36" s="97"/>
+      <c r="P36" s="97"/>
+      <c r="Q36" s="97"/>
+      <c r="R36" s="97"/>
     </row>
     <row r="37" spans="1:35" s="71" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A37" s="92" t="s">
+      <c r="A37" s="98" t="s">
         <v>964</v>
       </c>
       <c r="B37" s="77"/>
@@ -83139,7 +83123,7 @@
       <c r="R37" s="77"/>
     </row>
     <row r="38" spans="1:35" s="71" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A38" s="85" t="s">
+      <c r="A38" s="76" t="s">
         <v>965</v>
       </c>
       <c r="B38" s="77"/>
@@ -83161,7 +83145,7 @@
       <c r="R38" s="77"/>
     </row>
     <row r="39" spans="1:35" s="71" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A39" s="76" t="s">
+      <c r="A39" s="78" t="s">
         <v>966</v>
       </c>
       <c r="B39" s="77"/>
@@ -83183,7 +83167,7 @@
       <c r="R39" s="77"/>
     </row>
     <row r="40" spans="1:35" s="71" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A40" s="85" t="s">
+      <c r="A40" s="76" t="s">
         <v>967</v>
       </c>
       <c r="B40" s="77"/>
@@ -83205,7 +83189,7 @@
       <c r="R40" s="77"/>
     </row>
     <row r="41" spans="1:35" s="71" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A41" s="85" t="s">
+      <c r="A41" s="76" t="s">
         <v>968</v>
       </c>
       <c r="B41" s="77"/>
@@ -83227,7 +83211,7 @@
       <c r="R41" s="77"/>
     </row>
     <row r="42" spans="1:35" s="71" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A42" s="85" t="s">
+      <c r="A42" s="76" t="s">
         <v>969</v>
       </c>
       <c r="B42" s="77"/>
@@ -83249,7 +83233,7 @@
       <c r="R42" s="77"/>
     </row>
     <row r="43" spans="1:35" s="71" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A43" s="76" t="s">
+      <c r="A43" s="78" t="s">
         <v>970</v>
       </c>
       <c r="B43" s="77"/>
@@ -83271,7 +83255,7 @@
       <c r="R43" s="77"/>
     </row>
     <row r="44" spans="1:35" s="71" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A44" s="76" t="s">
+      <c r="A44" s="78" t="s">
         <v>971</v>
       </c>
       <c r="B44" s="77"/>
@@ -83293,7 +83277,7 @@
       <c r="R44" s="77"/>
     </row>
     <row r="45" spans="1:35" s="71" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A45" s="97" t="s">
+      <c r="A45" s="79" t="s">
         <v>972</v>
       </c>
       <c r="B45" s="77"/>
@@ -83315,7 +83299,7 @@
       <c r="R45" s="77"/>
     </row>
     <row r="46" spans="1:35" s="71" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A46" s="85" t="s">
+      <c r="A46" s="76" t="s">
         <v>973</v>
       </c>
       <c r="B46" s="77"/>
@@ -83337,7 +83321,7 @@
       <c r="R46" s="77"/>
     </row>
     <row r="47" spans="1:35" s="71" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A47" s="85" t="s">
+      <c r="A47" s="76" t="s">
         <v>974</v>
       </c>
       <c r="B47" s="77"/>
@@ -83359,7 +83343,7 @@
       <c r="R47" s="77"/>
     </row>
     <row r="48" spans="1:35" s="71" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A48" s="85" t="s">
+      <c r="A48" s="76" t="s">
         <v>975</v>
       </c>
       <c r="B48" s="77"/>
@@ -83381,7 +83365,7 @@
       <c r="R48" s="77"/>
     </row>
     <row r="49" spans="1:18" s="71" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A49" s="85" t="s">
+      <c r="A49" s="76" t="s">
         <v>976</v>
       </c>
       <c r="B49" s="77"/>
@@ -83403,7 +83387,7 @@
       <c r="R49" s="77"/>
     </row>
     <row r="50" spans="1:18" s="71" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A50" s="85" t="s">
+      <c r="A50" s="76" t="s">
         <v>977</v>
       </c>
       <c r="B50" s="77"/>
@@ -83423,7 +83407,7 @@
       <c r="P50" s="77"/>
     </row>
     <row r="51" spans="1:18" s="71" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A51" s="78"/>
+      <c r="A51" s="99"/>
       <c r="B51" s="77"/>
       <c r="C51" s="77"/>
       <c r="D51" s="77"/>
@@ -83441,7 +83425,7 @@
       <c r="P51" s="77"/>
     </row>
     <row r="52" spans="1:18" s="71" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A52" s="96" t="s">
+      <c r="A52" s="88" t="s">
         <v>978</v>
       </c>
       <c r="B52" s="77"/>
@@ -83461,7 +83445,7 @@
       <c r="P52" s="77"/>
     </row>
     <row r="53" spans="1:18" s="71" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A53" s="97" t="s">
+      <c r="A53" s="79" t="s">
         <v>979</v>
       </c>
       <c r="B53" s="77"/>
@@ -83481,7 +83465,7 @@
       <c r="P53" s="77"/>
     </row>
     <row r="54" spans="1:18" s="71" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A54" s="79" t="s">
+      <c r="A54" s="81" t="s">
         <v>980</v>
       </c>
       <c r="B54" s="77"/>
@@ -83501,7 +83485,7 @@
       <c r="P54" s="77"/>
     </row>
     <row r="55" spans="1:18" s="71" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A55" s="81" t="s">
+      <c r="A55" s="100" t="s">
         <v>981</v>
       </c>
       <c r="B55" s="77"/>
@@ -83521,7 +83505,7 @@
       <c r="P55" s="77"/>
     </row>
     <row r="56" spans="1:18" s="71" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A56" s="79" t="s">
+      <c r="A56" s="81" t="s">
         <v>982</v>
       </c>
       <c r="B56" s="77"/>
@@ -83541,7 +83525,7 @@
       <c r="P56" s="77"/>
     </row>
     <row r="57" spans="1:18" s="71" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A57" s="79" t="s">
+      <c r="A57" s="81" t="s">
         <v>983</v>
       </c>
       <c r="B57" s="77"/>
@@ -83561,7 +83545,7 @@
       <c r="P57" s="77"/>
     </row>
     <row r="58" spans="1:18" s="71" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A58" s="98" t="s">
+      <c r="A58" s="89" t="s">
         <v>984</v>
       </c>
       <c r="B58" s="77"/>
@@ -83581,7 +83565,7 @@
       <c r="P58" s="77"/>
     </row>
     <row r="59" spans="1:18" s="71" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A59" s="83"/>
+      <c r="A59" s="101"/>
       <c r="B59" s="77"/>
       <c r="C59" s="77"/>
       <c r="D59" s="77"/>
@@ -83659,7 +83643,7 @@
       <c r="P62" s="77"/>
     </row>
     <row r="63" spans="1:18" s="71" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A63" s="99" t="s">
+      <c r="A63" s="91" t="s">
         <v>988</v>
       </c>
       <c r="B63" s="77"/>
@@ -83879,7 +83863,7 @@
       <c r="P73" s="77"/>
     </row>
     <row r="74" spans="1:16" s="71" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A74" s="82" t="s">
+      <c r="A74" s="86" t="s">
         <v>999</v>
       </c>
       <c r="B74" s="77"/>
@@ -83919,7 +83903,7 @@
       <c r="P75" s="77"/>
     </row>
     <row r="76" spans="1:16" s="71" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A76" s="79" t="s">
+      <c r="A76" s="81" t="s">
         <v>1001</v>
       </c>
       <c r="B76" s="77"/>
@@ -83939,7 +83923,7 @@
       <c r="P76" s="77"/>
     </row>
     <row r="77" spans="1:16" s="71" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A77" s="95" t="s">
+      <c r="A77" s="85" t="s">
         <v>1002</v>
       </c>
       <c r="B77" s="77"/>
@@ -83959,7 +83943,7 @@
       <c r="P77" s="77"/>
     </row>
     <row r="78" spans="1:16" s="71" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A78" s="94" t="s">
+      <c r="A78" s="87" t="s">
         <v>1003</v>
       </c>
       <c r="B78" s="77"/>
@@ -83979,7 +83963,7 @@
       <c r="P78" s="77"/>
     </row>
     <row r="79" spans="1:16" s="71" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A79" s="95" t="s">
+      <c r="A79" s="85" t="s">
         <v>1004</v>
       </c>
       <c r="B79" s="77"/>
@@ -84019,7 +84003,7 @@
       <c r="P80" s="77"/>
     </row>
     <row r="81" spans="1:16" s="71" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A81" s="79" t="s">
+      <c r="A81" s="81" t="s">
         <v>1006</v>
       </c>
       <c r="B81" s="77"/>
@@ -84039,7 +84023,7 @@
       <c r="P81" s="77"/>
     </row>
     <row r="82" spans="1:16" s="71" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A82" s="95" t="s">
+      <c r="A82" s="85" t="s">
         <v>1007</v>
       </c>
       <c r="B82" s="77"/>
@@ -84079,7 +84063,7 @@
       <c r="P83" s="77"/>
     </row>
     <row r="84" spans="1:16" s="71" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A84" s="79" t="s">
+      <c r="A84" s="81" t="s">
         <v>1009</v>
       </c>
       <c r="B84" s="77"/>
@@ -84099,7 +84083,7 @@
       <c r="P84" s="77"/>
     </row>
     <row r="85" spans="1:16" s="71" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A85" s="95" t="s">
+      <c r="A85" s="85" t="s">
         <v>1002</v>
       </c>
       <c r="B85" s="77"/>
@@ -84119,7 +84103,7 @@
       <c r="P85" s="77"/>
     </row>
     <row r="86" spans="1:16" s="71" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A86" s="94" t="s">
+      <c r="A86" s="87" t="s">
         <v>1010</v>
       </c>
       <c r="B86" s="77"/>
@@ -84139,7 +84123,7 @@
       <c r="P86" s="77"/>
     </row>
     <row r="87" spans="1:16" s="71" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A87" s="95" t="s">
+      <c r="A87" s="85" t="s">
         <v>1004</v>
       </c>
       <c r="B87" s="77"/>
@@ -84179,7 +84163,7 @@
       <c r="P88" s="77"/>
     </row>
     <row r="89" spans="1:16" s="71" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A89" s="79" t="s">
+      <c r="A89" s="81" t="s">
         <v>1012</v>
       </c>
       <c r="B89" s="77"/>
@@ -84199,7 +84183,7 @@
       <c r="P89" s="77"/>
     </row>
     <row r="90" spans="1:16" s="71" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A90" s="95" t="s">
+      <c r="A90" s="85" t="s">
         <v>1007</v>
       </c>
       <c r="B90" s="77"/>
@@ -84219,7 +84203,7 @@
       <c r="P90" s="77"/>
     </row>
     <row r="91" spans="1:16" s="71" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A91" s="82" t="s">
+      <c r="A91" s="86" t="s">
         <v>1013</v>
       </c>
       <c r="B91" s="77"/>
@@ -84299,7 +84283,7 @@
       <c r="P94" s="77"/>
     </row>
     <row r="95" spans="1:16" s="71" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A95" s="82" t="s">
+      <c r="A95" s="86" t="s">
         <v>1017</v>
       </c>
       <c r="B95" s="77"/>
@@ -84342,24 +84326,24 @@
       <c r="A97" s="80" t="s">
         <v>1018</v>
       </c>
-      <c r="B97" s="93"/>
-      <c r="C97" s="93"/>
-      <c r="D97" s="93"/>
-      <c r="E97" s="93"/>
-      <c r="F97" s="93"/>
-      <c r="G97" s="93"/>
-      <c r="H97" s="93"/>
-      <c r="I97" s="93"/>
-      <c r="J97" s="93"/>
-      <c r="K97" s="93"/>
-      <c r="L97" s="93"/>
-      <c r="M97" s="93"/>
-      <c r="N97" s="93"/>
-      <c r="O97" s="93"/>
-      <c r="P97" s="93"/>
+      <c r="B97" s="92"/>
+      <c r="C97" s="92"/>
+      <c r="D97" s="92"/>
+      <c r="E97" s="92"/>
+      <c r="F97" s="92"/>
+      <c r="G97" s="92"/>
+      <c r="H97" s="92"/>
+      <c r="I97" s="92"/>
+      <c r="J97" s="92"/>
+      <c r="K97" s="92"/>
+      <c r="L97" s="92"/>
+      <c r="M97" s="92"/>
+      <c r="N97" s="92"/>
+      <c r="O97" s="92"/>
+      <c r="P97" s="92"/>
     </row>
     <row r="98" spans="1:20" s="71" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A98" s="82" t="s">
+      <c r="A98" s="86" t="s">
         <v>1019</v>
       </c>
       <c r="B98" s="77"/>
@@ -84459,7 +84443,7 @@
       <c r="P102" s="77"/>
     </row>
     <row r="103" spans="1:20" s="71" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A103" s="82" t="s">
+      <c r="A103" s="86" t="s">
         <v>1024</v>
       </c>
       <c r="B103" s="77"/>
@@ -84499,7 +84483,7 @@
       <c r="P104" s="77"/>
     </row>
     <row r="105" spans="1:20" s="71" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A105" s="79" t="s">
+      <c r="A105" s="81" t="s">
         <v>1026</v>
       </c>
       <c r="B105" s="77"/>
@@ -84519,7 +84503,7 @@
       <c r="P105" s="77"/>
     </row>
     <row r="106" spans="1:20" s="71" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A106" s="79" t="s">
+      <c r="A106" s="81" t="s">
         <v>1027</v>
       </c>
       <c r="B106" s="77"/>
@@ -84559,7 +84543,7 @@
       <c r="P107" s="77"/>
     </row>
     <row r="108" spans="1:20" s="71" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A108" s="100" t="s">
+      <c r="A108" s="82" t="s">
         <v>1029</v>
       </c>
       <c r="B108" s="77"/>
@@ -84579,7 +84563,7 @@
       <c r="P108" s="77"/>
     </row>
     <row r="109" spans="1:20" s="71" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A109" s="101" t="s">
+      <c r="A109" s="83" t="s">
         <v>1030</v>
       </c>
       <c r="B109" s="77"/>
@@ -84696,15 +84680,59 @@
     </row>
   </sheetData>
   <mergeCells count="78">
-    <mergeCell ref="A46:R46"/>
-    <mergeCell ref="A47:R47"/>
-    <mergeCell ref="A48:R48"/>
-    <mergeCell ref="A49:R49"/>
-    <mergeCell ref="A41:R41"/>
-    <mergeCell ref="A42:R42"/>
-    <mergeCell ref="A43:R43"/>
-    <mergeCell ref="A44:R44"/>
-    <mergeCell ref="A45:R45"/>
+    <mergeCell ref="A39:R39"/>
+    <mergeCell ref="A51:P51"/>
+    <mergeCell ref="A76:P76"/>
+    <mergeCell ref="A70:P70"/>
+    <mergeCell ref="A65:P65"/>
+    <mergeCell ref="A55:P55"/>
+    <mergeCell ref="A56:P56"/>
+    <mergeCell ref="A57:P57"/>
+    <mergeCell ref="A71:P71"/>
+    <mergeCell ref="A72:P72"/>
+    <mergeCell ref="A73:P73"/>
+    <mergeCell ref="A74:P74"/>
+    <mergeCell ref="A69:P69"/>
+    <mergeCell ref="A59:P59"/>
+    <mergeCell ref="A75:P75"/>
+    <mergeCell ref="A40:R40"/>
+    <mergeCell ref="A1:AI1"/>
+    <mergeCell ref="A35:R35"/>
+    <mergeCell ref="A36:R36"/>
+    <mergeCell ref="A37:R37"/>
+    <mergeCell ref="A38:R38"/>
+    <mergeCell ref="A107:P107"/>
+    <mergeCell ref="A100:P100"/>
+    <mergeCell ref="A97:P97"/>
+    <mergeCell ref="A99:P99"/>
+    <mergeCell ref="A96:P96"/>
+    <mergeCell ref="A98:P98"/>
+    <mergeCell ref="A101:P101"/>
+    <mergeCell ref="A78:P78"/>
+    <mergeCell ref="A79:P79"/>
+    <mergeCell ref="A80:P80"/>
+    <mergeCell ref="A52:P52"/>
+    <mergeCell ref="A53:P53"/>
+    <mergeCell ref="A58:P58"/>
+    <mergeCell ref="A54:P54"/>
+    <mergeCell ref="A77:P77"/>
+    <mergeCell ref="A60:P60"/>
+    <mergeCell ref="A61:P61"/>
+    <mergeCell ref="A62:P62"/>
+    <mergeCell ref="A63:P63"/>
+    <mergeCell ref="A64:P64"/>
+    <mergeCell ref="A66:P66"/>
+    <mergeCell ref="A67:P67"/>
+    <mergeCell ref="A68:P68"/>
+    <mergeCell ref="A89:P89"/>
+    <mergeCell ref="A90:P90"/>
+    <mergeCell ref="A95:P95"/>
+    <mergeCell ref="A81:P81"/>
+    <mergeCell ref="A82:P82"/>
+    <mergeCell ref="A84:P84"/>
+    <mergeCell ref="A85:P85"/>
+    <mergeCell ref="A86:P86"/>
+    <mergeCell ref="A83:P83"/>
     <mergeCell ref="A111:P111"/>
     <mergeCell ref="A50:P50"/>
     <mergeCell ref="A92:P92"/>
@@ -84721,59 +84749,15 @@
     <mergeCell ref="A103:P103"/>
     <mergeCell ref="A104:P104"/>
     <mergeCell ref="A91:P91"/>
-    <mergeCell ref="A89:P89"/>
-    <mergeCell ref="A90:P90"/>
-    <mergeCell ref="A95:P95"/>
-    <mergeCell ref="A81:P81"/>
-    <mergeCell ref="A82:P82"/>
-    <mergeCell ref="A84:P84"/>
-    <mergeCell ref="A85:P85"/>
-    <mergeCell ref="A86:P86"/>
-    <mergeCell ref="A83:P83"/>
-    <mergeCell ref="A78:P78"/>
-    <mergeCell ref="A79:P79"/>
-    <mergeCell ref="A80:P80"/>
-    <mergeCell ref="A52:P52"/>
-    <mergeCell ref="A53:P53"/>
-    <mergeCell ref="A58:P58"/>
-    <mergeCell ref="A54:P54"/>
-    <mergeCell ref="A77:P77"/>
-    <mergeCell ref="A60:P60"/>
-    <mergeCell ref="A61:P61"/>
-    <mergeCell ref="A62:P62"/>
-    <mergeCell ref="A63:P63"/>
-    <mergeCell ref="A64:P64"/>
-    <mergeCell ref="A66:P66"/>
-    <mergeCell ref="A67:P67"/>
-    <mergeCell ref="A68:P68"/>
-    <mergeCell ref="A107:P107"/>
-    <mergeCell ref="A100:P100"/>
-    <mergeCell ref="A97:P97"/>
-    <mergeCell ref="A99:P99"/>
-    <mergeCell ref="A96:P96"/>
-    <mergeCell ref="A98:P98"/>
-    <mergeCell ref="A101:P101"/>
-    <mergeCell ref="A1:AI1"/>
-    <mergeCell ref="A35:R35"/>
-    <mergeCell ref="A36:R36"/>
-    <mergeCell ref="A37:R37"/>
-    <mergeCell ref="A38:R38"/>
-    <mergeCell ref="A39:R39"/>
-    <mergeCell ref="A51:P51"/>
-    <mergeCell ref="A76:P76"/>
-    <mergeCell ref="A70:P70"/>
-    <mergeCell ref="A65:P65"/>
-    <mergeCell ref="A55:P55"/>
-    <mergeCell ref="A56:P56"/>
-    <mergeCell ref="A57:P57"/>
-    <mergeCell ref="A71:P71"/>
-    <mergeCell ref="A72:P72"/>
-    <mergeCell ref="A73:P73"/>
-    <mergeCell ref="A74:P74"/>
-    <mergeCell ref="A69:P69"/>
-    <mergeCell ref="A59:P59"/>
-    <mergeCell ref="A75:P75"/>
-    <mergeCell ref="A40:R40"/>
+    <mergeCell ref="A46:R46"/>
+    <mergeCell ref="A47:R47"/>
+    <mergeCell ref="A48:R48"/>
+    <mergeCell ref="A49:R49"/>
+    <mergeCell ref="A41:R41"/>
+    <mergeCell ref="A42:R42"/>
+    <mergeCell ref="A43:R43"/>
+    <mergeCell ref="A44:R44"/>
+    <mergeCell ref="A45:R45"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="35" fitToHeight="0" orientation="landscape"/>

</xml_diff>